<commit_message>
CV liquidación de compra, reportes, pantalla con retenciones
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-LiqCompras.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-LiqCompras.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90BA37-2480-0045-AE0F-C250593DA30C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3075937D-D3CE-8744-BE37-D0B51044FD2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="10020" windowWidth="35960" windowHeight="18240" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
+    <workbookView xWindow="14140" yWindow="8160" windowWidth="44260" windowHeight="19720" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>% IVA</t>
   </si>
@@ -42,18 +42,9 @@
     <t>HASTA:</t>
   </si>
   <si>
-    <t>N.</t>
-  </si>
-  <si>
-    <t>FECHA EMISIÓN</t>
-  </si>
-  <si>
     <t>ESTADO</t>
   </si>
   <si>
-    <t>AUT S.R.I.</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -66,15 +57,6 @@
     <t>PAGO</t>
   </si>
   <si>
-    <t>ENTREGA</t>
-  </si>
-  <si>
-    <t>CAMBIO</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
     <t>TOT SIN IMPU</t>
   </si>
   <si>
@@ -84,41 +66,26 @@
     <t>PROVEEDOR</t>
   </si>
   <si>
-    <t>NUM DOC</t>
-  </si>
-  <si>
-    <t>BANCO</t>
-  </si>
-  <si>
     <t>LIQUIDACIÓN DE COMPRAS EMITIDAS</t>
   </si>
   <si>
-    <t>ITEM</t>
-  </si>
-  <si>
-    <t>PRE UNIT</t>
-  </si>
-  <si>
-    <t>I.V.A.</t>
-  </si>
-  <si>
-    <t>LIQUIDACIÓN DE COMPRA</t>
-  </si>
-  <si>
-    <t>DETALLE</t>
-  </si>
-  <si>
-    <t>PAGOS</t>
-  </si>
-  <si>
-    <t>VALOR</t>
+    <t>NUM COMP</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>RETENCIÓN</t>
+  </si>
+  <si>
+    <t>A PAGAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,13 +100,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -191,25 +151,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,33 +480,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:X10"/>
+  <dimension ref="A2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="12" width="40" customWidth="1"/>
-    <col min="13" max="19" width="13.5" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" customWidth="1"/>
-    <col min="22" max="22" width="16.33203125" customWidth="1"/>
+    <col min="2" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -566,174 +517,91 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="M9" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="L9:R9"/>
-    <mergeCell ref="S9:X9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A2:X2"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>